<commit_message>
same data but using different locations
</commit_message>
<xml_diff>
--- a/shinyapp/data/school_locations.xlsx
+++ b/shinyapp/data/school_locations.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amandaljuba/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nandinidas/Desktop/2022_DSPG_Loudoun/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3ABFE2D5-928B-7048-8E98-FC8DF594AFA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6321967B-B707-7C42-829B-CC26DCA0505E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9260" yWindow="1920" windowWidth="14800" windowHeight="8020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{2DE02477-F050-8A47-B147-A7F0C5BFB2F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -43,12 +46,6 @@
     <t>Coordinates</t>
   </si>
   <si>
-    <t>Latitudes</t>
-  </si>
-  <si>
-    <t>Longitudes</t>
-  </si>
-  <si>
     <t>Sterling Elementary</t>
   </si>
   <si>
@@ -101,16 +98,29 @@
   </si>
   <si>
     <t xml:space="preserve">                                                              </t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -127,6 +137,7 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -153,13 +164,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -467,118 +478,111 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83AB6A0E-DB43-8F4B-9368-8E9D156565C1}">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="23.83203125" customWidth="1"/>
-    <col min="2" max="2" width="33" customWidth="1"/>
-    <col min="3" max="3" width="25.5" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>39.009005999999999</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>-77.402915500000006</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="D3" s="3">
         <v>38.996525099999999</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="3">
         <v>-77.398243500000007</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="2">
+      <c r="D4" s="3">
         <v>38.994751999999998</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="3">
         <v>-77.408112000000003</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="D5" s="3">
         <v>39.036763100000002</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="3">
         <v>-77.382812299999998</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="2">
+      <c r="D6" s="3">
         <v>39.015029499999997</v>
       </c>
       <c r="E6" s="3">
@@ -586,318 +590,23 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="2">
+      <c r="D7" s="3">
         <v>38.990546000000002</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="3">
         <v>-77.399018999999996</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="cf6ddc61-6b1c-4d58-9daa-562ef749da72" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d3dcd26c-518f-4103-85e3-288a7f67eda7">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008E8A14C35611B44FAE08C7282FBC43BB" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f8c258f84c8883adaba6693857568905">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d3dcd26c-518f-4103-85e3-288a7f67eda7" xmlns:ns3="cf6ddc61-6b1c-4d58-9daa-562ef749da72" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b6e5ccfb7e00e6117bade8c94a8a5e1" ns2:_="" ns3:_="">
-    <xsd:import namespace="d3dcd26c-518f-4103-85e3-288a7f67eda7"/>
-    <xsd:import namespace="cf6ddc61-6b1c-4d58-9daa-562ef749da72"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
-                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
-                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="d3dcd26c-518f-4103-85e3-288a7f67eda7" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="10" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="11" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoTags" ma:index="12" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="13" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="19" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="886477d7-ad29-47e7-b319-eaa6f1949674" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="21" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceKeyPoints" ma:index="22" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="cf6ddc61-6b1c-4d58-9daa-562ef749da72" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="16" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:UserMulti">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="17" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TaxCatchAll" ma:index="20" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{205a5ac6-0c3d-42f9-b046-9f2a27b47c85}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="cf6ddc61-6b1c-4d58-9daa-562ef749da72">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63E52F4A-4182-444B-9BD6-E8E43B29CEB9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cf6ddc61-6b1c-4d58-9daa-562ef749da72"/>
-    <ds:schemaRef ds:uri="d3dcd26c-518f-4103-85e3-288a7f67eda7"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4FF1D4DD-6813-46BE-8851-8B6F8F05049B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="d3dcd26c-518f-4103-85e3-288a7f67eda7"/>
-    <ds:schemaRef ds:uri="cf6ddc61-6b1c-4d58-9daa-562ef749da72"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11D8F160-570E-49E0-9431-C70F397DA65D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
i hope i didnt mess it up
</commit_message>
<xml_diff>
--- a/shinyapp/data/school_locations.xlsx
+++ b/shinyapp/data/school_locations.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amandaljuba/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nandinidas/Desktop/2022_DSPG_Loudoun/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3ABFE2D5-928B-7048-8E98-FC8DF594AFA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6321967B-B707-7C42-829B-CC26DCA0505E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9260" yWindow="1920" windowWidth="14800" windowHeight="8020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{2DE02477-F050-8A47-B147-A7F0C5BFB2F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -43,12 +46,6 @@
     <t>Coordinates</t>
   </si>
   <si>
-    <t>Latitudes</t>
-  </si>
-  <si>
-    <t>Longitudes</t>
-  </si>
-  <si>
     <t>Sterling Elementary</t>
   </si>
   <si>
@@ -101,16 +98,29 @@
   </si>
   <si>
     <t xml:space="preserve">                                                              </t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF333333"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -127,6 +137,7 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -153,13 +164,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -467,118 +478,111 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83AB6A0E-DB43-8F4B-9368-8E9D156565C1}">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="23.83203125" customWidth="1"/>
-    <col min="2" max="2" width="33" customWidth="1"/>
-    <col min="3" max="3" width="25.5" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2">
+      <c r="D2" s="1">
         <v>39.009005999999999</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>-77.402915500000006</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="2">
+      <c r="D3" s="3">
         <v>38.996525099999999</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="3">
         <v>-77.398243500000007</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="2">
+      <c r="D4" s="3">
         <v>38.994751999999998</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="3">
         <v>-77.408112000000003</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="2">
+      <c r="D5" s="3">
         <v>39.036763100000002</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="3">
         <v>-77.382812299999998</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-      <c r="D6" s="2">
+      <c r="D6" s="3">
         <v>39.015029499999997</v>
       </c>
       <c r="E6" s="3">
@@ -586,318 +590,23 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="2">
+      <c r="D7" s="3">
         <v>38.990546000000002</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="3">
         <v>-77.399018999999996</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="cf6ddc61-6b1c-4d58-9daa-562ef749da72" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d3dcd26c-518f-4103-85e3-288a7f67eda7">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008E8A14C35611B44FAE08C7282FBC43BB" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f8c258f84c8883adaba6693857568905">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d3dcd26c-518f-4103-85e3-288a7f67eda7" xmlns:ns3="cf6ddc61-6b1c-4d58-9daa-562ef749da72" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8b6e5ccfb7e00e6117bade8c94a8a5e1" ns2:_="" ns3:_="">
-    <xsd:import namespace="d3dcd26c-518f-4103-85e3-288a7f67eda7"/>
-    <xsd:import namespace="cf6ddc61-6b1c-4d58-9daa-562ef749da72"/>
-    <xsd:element name="properties">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element name="documentManagement">
-            <xsd:complexType>
-              <xsd:all>
-                <xsd:element ref="ns2:MediaServiceMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
-                <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
-                <xsd:element ref="ns2:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
-                <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
-                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
-              </xsd:all>
-            </xsd:complexType>
-          </xsd:element>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="d3dcd26c-518f-4103-85e3-288a7f67eda7" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="MediaServiceMetadata" ma:index="8" nillable="true" ma:displayName="MediaServiceMetadata" ma:hidden="true" ma:internalName="MediaServiceMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceDateTaken" ma:index="10" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaLengthInSeconds" ma:index="11" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Unknown"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoTags" ma:index="12" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceOCR" ma:index="13" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceGenerationTime" ma:index="14" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceEventHashCode" ma:index="15" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Text"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="19" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="886477d7-ad29-47e7-b319-eaa6f1949674" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
-      <xsd:complexType>
-        <xsd:sequence>
-          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
-        </xsd:sequence>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="21" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note"/>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="MediaServiceKeyPoints" ma:index="22" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:dms="http://schemas.microsoft.com/office/2006/documentManagement/types" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" targetNamespace="cf6ddc61-6b1c-4d58-9daa-562ef749da72" elementFormDefault="qualified">
-    <xsd:import namespace="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <xsd:import namespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <xsd:element name="SharedWithUsers" ma:index="16" nillable="true" ma:displayName="Shared With" ma:internalName="SharedWithUsers" ma:readOnly="true">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:UserMulti">
-            <xsd:sequence>
-              <xsd:element name="UserInfo" minOccurs="0" maxOccurs="unbounded">
-                <xsd:complexType>
-                  <xsd:sequence>
-                    <xsd:element name="DisplayName" type="xsd:string" minOccurs="0"/>
-                    <xsd:element name="AccountId" type="dms:UserId" minOccurs="0" nillable="true"/>
-                    <xsd:element name="AccountType" type="xsd:string" minOccurs="0"/>
-                  </xsd:sequence>
-                </xsd:complexType>
-              </xsd:element>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-    <xsd:element name="SharedWithDetails" ma:index="17" nillable="true" ma:displayName="Shared With Details" ma:internalName="SharedWithDetails" ma:readOnly="true">
-      <xsd:simpleType>
-        <xsd:restriction base="dms:Note">
-          <xsd:maxLength value="255"/>
-        </xsd:restriction>
-      </xsd:simpleType>
-    </xsd:element>
-    <xsd:element name="TaxCatchAll" ma:index="20" nillable="true" ma:displayName="Taxonomy Catch All Column" ma:hidden="true" ma:list="{205a5ac6-0c3d-42f9-b046-9f2a27b47c85}" ma:internalName="TaxCatchAll" ma:showField="CatchAllData" ma:web="cf6ddc61-6b1c-4d58-9daa-562ef749da72">
-      <xsd:complexType>
-        <xsd:complexContent>
-          <xsd:extension base="dms:MultiChoiceLookup">
-            <xsd:sequence>
-              <xsd:element name="Value" type="dms:Lookup" maxOccurs="unbounded" minOccurs="0" nillable="true"/>
-            </xsd:sequence>
-          </xsd:extension>
-        </xsd:complexContent>
-      </xsd:complexType>
-    </xsd:element>
-  </xsd:schema>
-  <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
-    <xsd:import namespace="http://purl.org/dc/elements/1.1/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dc.xsd"/>
-    <xsd:import namespace="http://purl.org/dc/terms/" schemaLocation="http://dublincore.org/schemas/xmls/qdc/2003/04/02/dcterms.xsd"/>
-    <xsd:element name="coreProperties" type="CT_coreProperties"/>
-    <xsd:complexType name="CT_coreProperties">
-      <xsd:all>
-        <xsd:element ref="dc:creator" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dcterms:created" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:identifier" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentType" minOccurs="0" maxOccurs="1" type="xsd:string" ma:index="0" ma:displayName="Content Type"/>
-        <xsd:element ref="dc:title" minOccurs="0" maxOccurs="1" ma:index="4" ma:displayName="Title"/>
-        <xsd:element ref="dc:subject" minOccurs="0" maxOccurs="1"/>
-        <xsd:element ref="dc:description" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="keywords" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dc:language" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="category" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="version" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element name="revision" minOccurs="0" maxOccurs="1" type="xsd:string">
-          <xsd:annotation>
-            <xsd:documentation>
-                        This value indicates the number of saves or revisions. The application is responsible for updating this value after each revision.
-                    </xsd:documentation>
-          </xsd:annotation>
-        </xsd:element>
-        <xsd:element name="lastModifiedBy" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-        <xsd:element ref="dcterms:modified" minOccurs="0" maxOccurs="1"/>
-        <xsd:element name="contentStatus" minOccurs="0" maxOccurs="1" type="xsd:string"/>
-      </xsd:all>
-    </xsd:complexType>
-  </xsd:schema>
-  <xs:schema xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" xmlns:xs="http://www.w3.org/2001/XMLSchema" targetNamespace="http://schemas.microsoft.com/office/infopath/2007/PartnerControls" elementFormDefault="qualified" attributeFormDefault="unqualified">
-    <xs:element name="Person">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:DisplayName" minOccurs="0"/>
-          <xs:element ref="pc:AccountId" minOccurs="0"/>
-          <xs:element ref="pc:AccountType" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="DisplayName" type="xs:string"/>
-    <xs:element name="AccountId" type="xs:string"/>
-    <xs:element name="AccountType" type="xs:string"/>
-    <xs:element name="BDCAssociatedEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:BDCEntity" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-        <xs:attribute ref="pc:EntityNamespace"/>
-        <xs:attribute ref="pc:EntityName"/>
-        <xs:attribute ref="pc:SystemInstanceName"/>
-        <xs:attribute ref="pc:AssociationName"/>
-      </xs:complexType>
-    </xs:element>
-    <xs:attribute name="EntityNamespace" type="xs:string"/>
-    <xs:attribute name="EntityName" type="xs:string"/>
-    <xs:attribute name="SystemInstanceName" type="xs:string"/>
-    <xs:attribute name="AssociationName" type="xs:string"/>
-    <xs:element name="BDCEntity">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:EntityDisplayName" minOccurs="0"/>
-          <xs:element ref="pc:EntityInstanceReference" minOccurs="0"/>
-          <xs:element ref="pc:EntityId1" minOccurs="0"/>
-          <xs:element ref="pc:EntityId2" minOccurs="0"/>
-          <xs:element ref="pc:EntityId3" minOccurs="0"/>
-          <xs:element ref="pc:EntityId4" minOccurs="0"/>
-          <xs:element ref="pc:EntityId5" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="EntityDisplayName" type="xs:string"/>
-    <xs:element name="EntityInstanceReference" type="xs:string"/>
-    <xs:element name="EntityId1" type="xs:string"/>
-    <xs:element name="EntityId2" type="xs:string"/>
-    <xs:element name="EntityId3" type="xs:string"/>
-    <xs:element name="EntityId4" type="xs:string"/>
-    <xs:element name="EntityId5" type="xs:string"/>
-    <xs:element name="Terms">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermInfo" minOccurs="0" maxOccurs="unbounded"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermInfo">
-      <xs:complexType>
-        <xs:sequence>
-          <xs:element ref="pc:TermName" minOccurs="0"/>
-          <xs:element ref="pc:TermId" minOccurs="0"/>
-        </xs:sequence>
-      </xs:complexType>
-    </xs:element>
-    <xs:element name="TermName" type="xs:string"/>
-    <xs:element name="TermId" type="xs:string"/>
-  </xs:schema>
-</ct:contentTypeSchema>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{63E52F4A-4182-444B-9BD6-E8E43B29CEB9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="cf6ddc61-6b1c-4d58-9daa-562ef749da72"/>
-    <ds:schemaRef ds:uri="d3dcd26c-518f-4103-85e3-288a7f67eda7"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4FF1D4DD-6813-46BE-8851-8B6F8F05049B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="d3dcd26c-518f-4103-85e3-288a7f67eda7"/>
-    <ds:schemaRef ds:uri="cf6ddc61-6b1c-4d58-9daa-562ef749da72"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{11D8F160-570E-49E0-9431-C70F397DA65D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
changes in Sterling tab
</commit_message>
<xml_diff>
--- a/shinyapp/data/school_locations.xlsx
+++ b/shinyapp/data/school_locations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nandinidas/Desktop/2022_DSPG_Loudoun/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nandinidas/Desktop/2022_DSPG_Loudoun/shinyapp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6321967B-B707-7C42-829B-CC26DCA0505E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37861221-B399-C34A-93AB-A38B86727A8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{2DE02477-F050-8A47-B147-A7F0C5BFB2F7}"/>
   </bookViews>
@@ -35,10 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
-  <si>
-    <t>School</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Address</t>
   </si>
@@ -104,13 +101,37 @@
   </si>
   <si>
     <t>Longitude</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Website</t>
+  </si>
+  <si>
+    <t>https://www.lcps.org/forestgrove</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.lcps.org/guilford </t>
+  </si>
+  <si>
+    <t>https://www.lcps.org/rollingridge</t>
+  </si>
+  <si>
+    <t>https://www.lcps.org/sterlinges</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.lcps.org/sully </t>
+  </si>
+  <si>
+    <t>https://www.lcps.org/sugarland</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -139,6 +160,30 @@
       <charset val="1"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -157,16 +202,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="8"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -479,40 +532,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83AB6A0E-DB43-8F4B-9368-8E9D156565C1}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="D2" s="1">
         <v>39.009005999999999</v>
@@ -520,16 +576,19 @@
       <c r="E2" s="1">
         <v>-77.402915500000006</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="D3" s="3">
         <v>38.996525099999999</v>
@@ -537,16 +596,19 @@
       <c r="E3" s="3">
         <v>-77.398243500000007</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
       </c>
       <c r="D4" s="3">
         <v>38.994751999999998</v>
@@ -554,16 +616,19 @@
       <c r="E4" s="3">
         <v>-77.408112000000003</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>14</v>
       </c>
       <c r="D5" s="3">
         <v>39.036763100000002</v>
@@ -571,16 +636,19 @@
       <c r="E5" s="3">
         <v>-77.382812299999998</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="D6" s="3">
         <v>39.015029499999997</v>
@@ -588,16 +656,19 @@
       <c r="E6" s="3">
         <v>-77.384221699999998</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="D7" s="3">
         <v>38.990546000000002</v>
@@ -605,8 +676,37 @@
       <c r="E7" s="3">
         <v>-77.399018999999996</v>
       </c>
+      <c r="F7" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J13" s="6"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J14" s="6"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J15" s="6"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J16" s="6"/>
+    </row>
+    <row r="17" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J17" s="6"/>
+    </row>
+    <row r="18" spans="10:10" x14ac:dyDescent="0.2">
+      <c r="J18" s="6"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F7" r:id="rId1" xr:uid="{21843B34-E2B0-374A-A994-BADE10589183}"/>
+    <hyperlink ref="F4" r:id="rId2" xr:uid="{3FEF4084-D4D9-DF46-8495-88F991DE0B4D}"/>
+    <hyperlink ref="F6" r:id="rId3" xr:uid="{80755019-7CE7-F24A-8B0E-FAC8F50082DD}"/>
+    <hyperlink ref="F2" r:id="rId4" xr:uid="{DC062BC0-EC40-0640-9EF0-FAA42780B58E}"/>
+    <hyperlink ref="F3" r:id="rId5" xr:uid="{D39237D0-6F9F-8647-A480-BF3691C86EA1}"/>
+    <hyperlink ref="F5" r:id="rId6" xr:uid="{9A995166-1552-5C47-BD60-EDD0C93E193A}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>